<commit_message>
added obtained results, the fep.py code, and some gnuplot codes we won't use
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeconce-my.sharepoint.com/personal/basgonzalez_udec_cl/Documents/Doctorado/1_Solvation in FDES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeconce-my.sharepoint.com/personal/basgonzalez_udec_cl/Documents/Doctorado/1_Solvation in FDES/HFC_in_FDES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{3E07C256-6B22-AF4B-8CA9-3DE7F670C480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E839280-446D-4D49-90C0-59950AE0CEFA}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{3E07C256-6B22-AF4B-8CA9-3DE7F670C480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5973BA7-4FB2-044E-8D67-FCB569112703}"/>
   <bookViews>
     <workbookView xWindow="-48720" yWindow="-1540" windowWidth="37300" windowHeight="18940" xr2:uid="{166621FB-05D4-1A41-9AA3-7E85740CA14F}"/>
   </bookViews>
@@ -342,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,36 +419,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -470,9 +440,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,6 +450,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,10 +502,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -831,29 +824,29 @@
   <dimension ref="B1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="47"/>
+      <c r="G2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="J2" s="45"/>
+      <c r="H2" s="47"/>
+      <c r="J2" s="35"/>
       <c r="K2" t="s">
         <v>29</v>
       </c>
@@ -862,7 +855,7 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
@@ -881,11 +874,11 @@
       <c r="H3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="46"/>
+      <c r="J3" s="36"/>
       <c r="K3" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="P3" s="30" t="s">
         <v>22</v>
       </c>
     </row>
@@ -893,22 +886,22 @@
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="32">
         <v>5.4369441012710696E-3</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="32">
         <v>5.1967424004768998E-4</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="33">
         <v>0.111366659635514</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="34">
         <v>8.7727547349323292E-3</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="39">
         <v>2.8675158249133598E-2</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="34">
         <v>2.39052202985531E-3</v>
       </c>
       <c r="P4" t="s">
@@ -925,10 +918,10 @@
       <c r="D5" s="3">
         <v>9.9538410846021393E-3</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="37">
         <v>0.48188538660165903</v>
       </c>
-      <c r="F5" s="48">
+      <c r="F5" s="38">
         <v>3.6763659520711298E-2</v>
       </c>
       <c r="G5" s="1">
@@ -951,16 +944,16 @@
       <c r="D6" s="3">
         <v>2.6204770688447201E-2</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="37">
         <v>0.44010835853357699</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="38">
         <v>3.3153519732830802E-2</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="40">
         <v>0.372255641605438</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="38">
         <v>2.5499848163200198E-2</v>
       </c>
       <c r="P6" t="s">
@@ -983,10 +976,10 @@
       <c r="F7" s="4">
         <v>4.9314690191474199E-2</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="40">
         <v>0.61651422451549098</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="38">
         <v>4.3704752478283301E-2</v>
       </c>
       <c r="P7" t="s">
@@ -997,10 +990,10 @@
       <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="31">
         <v>6.7013519105114003</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="31">
         <v>0.43479190035847898</v>
       </c>
       <c r="E8" s="11">
@@ -1032,24 +1025,24 @@
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="14"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33" t="s">
+      <c r="E11" s="50"/>
+      <c r="F11" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="32" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="34"/>
-      <c r="K11" s="35" t="s">
+      <c r="I11" s="52"/>
+      <c r="K11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="37"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="47"/>
       <c r="P11" t="s">
         <v>32</v>
       </c>
@@ -1085,12 +1078,12 @@
       <c r="N12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="P12" s="49" t="s">
+      <c r="P12" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -1121,14 +1114,22 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="17"/>
+      <c r="D14" s="15">
+        <v>0.158</v>
+      </c>
+      <c r="E14" s="15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F14" s="29">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="G14" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="H14" s="15"/>
       <c r="I14" s="17"/>
       <c r="K14" s="29" t="s">
@@ -1139,14 +1140,22 @@
       <c r="N14" s="17"/>
     </row>
     <row r="15" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="17"/>
+      <c r="D15" s="15">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E15" s="15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0.01</v>
+      </c>
       <c r="H15" s="15"/>
       <c r="I15" s="17"/>
       <c r="K15" s="27" t="s">
@@ -1157,13 +1166,13 @@
       <c r="N15" s="21"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="16">
         <v>0.376</v>
       </c>
       <c r="E16" s="15">
@@ -1179,7 +1188,7 @@
       <c r="I16" s="17"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="17" t="s">
         <v>12</v>
       </c>
@@ -1189,7 +1198,7 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="G17" s="17">
-        <v>5.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H17" s="15">
         <v>0.41299999999999998</v>
@@ -1199,7 +1208,7 @@
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="30"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="17" t="s">
         <v>13</v>
       </c>
@@ -1209,10 +1218,10 @@
       <c r="E18" s="18">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="41">
         <v>0.30299999999999999</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="42">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="H18" s="16">
@@ -1223,7 +1232,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -1237,7 +1246,7 @@
       <c r="I19" s="17"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="17" t="s">
         <v>12</v>
       </c>
@@ -1249,7 +1258,7 @@
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="21" t="s">
         <v>13</v>
       </c>
@@ -1262,17 +1271,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="K11:N11"/>
     <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>